<commit_message>
prototype features in place with onchange -> alert
</commit_message>
<xml_diff>
--- a/estimates.xlsx
+++ b/estimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\snippets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818BF1BE-6721-49BA-82E7-336E98F0E19E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956523C5-5AB7-4EA9-9FCA-520068B84FDD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="907" yWindow="848" windowWidth="19523" windowHeight="11624" xr2:uid="{5060BF3D-DF5E-4139-907C-03337B193FF3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>html + bootstrap</t>
   </si>
@@ -39,9 +39,6 @@
     <t>file system issues</t>
   </si>
   <si>
-    <t>front-end mechanism</t>
-  </si>
-  <si>
     <t>ES6 modules</t>
   </si>
   <si>
@@ -121,6 +118,24 @@
   </si>
   <si>
     <t>Function constructor (including validation)</t>
+  </si>
+  <si>
+    <t>Exercises Combo</t>
+  </si>
+  <si>
+    <t>Display Page</t>
+  </si>
+  <si>
+    <t>Reduce Page size</t>
+  </si>
+  <si>
+    <t>Display review template</t>
+  </si>
+  <si>
+    <t>Display Features</t>
+  </si>
+  <si>
+    <t>front-end mechanism (Prototype)</t>
   </si>
 </sst>
 </file>
@@ -475,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C1D66B-7AC0-4665-9C64-C53AD8F3A8BA}">
-  <dimension ref="C1:E36"/>
+  <dimension ref="C1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -488,12 +503,12 @@
   <sheetData>
     <row r="1" spans="3:5" x14ac:dyDescent="0.45">
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -517,16 +532,15 @@
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E5">
-        <f>SUM(D6:D10)</f>
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -534,7 +548,7 @@
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -542,7 +556,7 @@
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -550,7 +564,7 @@
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -558,95 +572,98 @@
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>5</v>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12">
-        <v>7</v>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13">
-        <v>21</v>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
+      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15">
-        <v>8</v>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20">
         <v>8</v>
-      </c>
-      <c r="E16">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20">
-        <v>4</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E21">
         <v>16</v>
@@ -654,7 +671,7 @@
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C22" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D22">
         <v>4</v>
@@ -662,7 +679,7 @@
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C23" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D23">
         <v>4</v>
@@ -670,7 +687,7 @@
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C24" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D24">
         <v>4</v>
@@ -678,7 +695,7 @@
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C25" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D25">
         <v>4</v>
@@ -686,15 +703,15 @@
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E26">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C27" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D27">
         <v>4</v>
@@ -702,7 +719,7 @@
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C28" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D28">
         <v>4</v>
@@ -710,32 +727,72 @@
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31">
         <v>12</v>
       </c>
-      <c r="D29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30">
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E36">
-        <f>SUM(E2:E35)</f>
-        <v>116</v>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="E41">
+        <f>SUM(E2:E40)</f>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>